<commit_message>
Dialog update - added dialog control - declares and includes now all use the same string syntax - fixed a bug in stat initialization - moved all generic stat functions into StatUtils - moved some duplicate code from monster and player into actor - refactored hp5 regen and re-used the code for mp5 regen (and potentially other regen / ticking stats) - removed all auto sell code and syntax for now
</commit_message>
<xml_diff>
--- a/data/content/Stats.xlsx
+++ b/data/content/Stats.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\EndlessBattleFC\data\content\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="0" windowWidth="18000" windowHeight="20820"/>
+    <workbookView xWindow="11160" yWindow="0" windowWidth="18000" windowHeight="18240"/>
   </bookViews>
   <sheets>
     <sheet name="StatDefinition" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>name</t>
   </si>
@@ -288,6 +283,18 @@
   </si>
   <si>
     <t>displayString</t>
+  </si>
+  <si>
+    <t>mp5</t>
+  </si>
+  <si>
+    <t>mp5Mult</t>
+  </si>
+  <si>
+    <t>MP/5: {0}</t>
+  </si>
+  <si>
+    <t>MP/5 Multiplier: {0}%</t>
   </si>
 </sst>
 </file>
@@ -597,7 +604,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -605,13 +612,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S7" sqref="S7"/>
+      <selection pane="bottomRight" activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,9 +743,6 @@
       <c r="O2">
         <v>100</v>
       </c>
-      <c r="P2" t="b">
-        <v>1</v>
-      </c>
       <c r="Q2" t="s">
         <v>53</v>
       </c>
@@ -789,9 +793,6 @@
       <c r="O3">
         <v>100</v>
       </c>
-      <c r="P3" t="b">
-        <v>1</v>
-      </c>
       <c r="Q3" t="s">
         <v>60</v>
       </c>
@@ -842,6 +843,9 @@
       <c r="O4">
         <v>1</v>
       </c>
+      <c r="P4" t="b">
+        <v>1</v>
+      </c>
       <c r="Q4" t="s">
         <v>56</v>
       </c>
@@ -892,9 +896,6 @@
       <c r="O5">
         <v>5</v>
       </c>
-      <c r="P5" t="b">
-        <v>1</v>
-      </c>
       <c r="Q5" t="s">
         <v>52</v>
       </c>
@@ -945,6 +946,9 @@
       <c r="O6">
         <v>1</v>
       </c>
+      <c r="P6" t="b">
+        <v>1</v>
+      </c>
       <c r="Q6" t="s">
         <v>58</v>
       </c>
@@ -995,9 +999,6 @@
       <c r="O7">
         <v>10</v>
       </c>
-      <c r="P7" t="b">
-        <v>1</v>
-      </c>
       <c r="Q7" t="s">
         <v>54</v>
       </c>
@@ -1048,9 +1049,6 @@
       <c r="O8">
         <v>10</v>
       </c>
-      <c r="P8" t="b">
-        <v>1</v>
-      </c>
       <c r="Q8" t="s">
         <v>59</v>
       </c>
@@ -1101,13 +1099,16 @@
       <c r="O9">
         <v>1</v>
       </c>
+      <c r="P9" t="b">
+        <v>1</v>
+      </c>
       <c r="Q9" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1149,18 +1150,15 @@
         <v>1</v>
       </c>
       <c r="O10">
-        <v>1</v>
-      </c>
-      <c r="P10" t="b">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q10" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1208,12 +1206,12 @@
         <v>1</v>
       </c>
       <c r="Q11" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1258,12 +1256,12 @@
         <v>1</v>
       </c>
       <c r="Q12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1307,16 +1305,13 @@
       <c r="O13">
         <v>1</v>
       </c>
-      <c r="P13" t="b">
-        <v>1</v>
-      </c>
       <c r="Q13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1360,13 +1355,16 @@
       <c r="O14">
         <v>1</v>
       </c>
+      <c r="P14" t="b">
+        <v>1</v>
+      </c>
       <c r="Q14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1410,16 +1408,13 @@
       <c r="O15">
         <v>1</v>
       </c>
-      <c r="P15" t="b">
-        <v>1</v>
-      </c>
       <c r="Q15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1463,13 +1458,16 @@
       <c r="O16">
         <v>1</v>
       </c>
+      <c r="P16" t="b">
+        <v>1</v>
+      </c>
       <c r="Q16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1513,16 +1511,13 @@
       <c r="O17">
         <v>1</v>
       </c>
-      <c r="P17" t="b">
-        <v>1</v>
-      </c>
       <c r="Q17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1566,13 +1561,16 @@
       <c r="O18">
         <v>1</v>
       </c>
+      <c r="P18" t="b">
+        <v>1</v>
+      </c>
       <c r="Q18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1616,16 +1614,13 @@
       <c r="O19">
         <v>1</v>
       </c>
-      <c r="P19" t="b">
-        <v>1</v>
-      </c>
       <c r="Q19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1669,13 +1664,16 @@
       <c r="O20">
         <v>1</v>
       </c>
+      <c r="P20" t="b">
+        <v>1</v>
+      </c>
       <c r="Q20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1716,16 +1714,16 @@
       <c r="N21">
         <v>1</v>
       </c>
-      <c r="P21" t="b">
+      <c r="O21">
         <v>1</v>
       </c>
       <c r="Q21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1769,13 +1767,16 @@
       <c r="O22">
         <v>1</v>
       </c>
+      <c r="P22" t="b">
+        <v>1</v>
+      </c>
       <c r="Q22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1817,12 +1818,12 @@
         <v>1</v>
       </c>
       <c r="Q23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1866,13 +1867,16 @@
       <c r="O24">
         <v>1</v>
       </c>
+      <c r="P24" t="b">
+        <v>1</v>
+      </c>
       <c r="Q24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1913,16 +1917,13 @@
       <c r="N25">
         <v>1</v>
       </c>
-      <c r="P25" t="b">
-        <v>1</v>
-      </c>
       <c r="Q25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1966,13 +1967,16 @@
       <c r="O26">
         <v>1</v>
       </c>
+      <c r="P26" t="b">
+        <v>1</v>
+      </c>
       <c r="Q26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2013,16 +2017,13 @@
       <c r="N27">
         <v>1</v>
       </c>
-      <c r="O27">
-        <v>1</v>
-      </c>
       <c r="Q27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2063,13 +2064,19 @@
       <c r="N28">
         <v>1</v>
       </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28" t="b">
+        <v>1</v>
+      </c>
       <c r="Q28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2113,13 +2120,16 @@
       <c r="O29">
         <v>1</v>
       </c>
+      <c r="P29" t="b">
+        <v>1</v>
+      </c>
       <c r="Q29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -2160,19 +2170,13 @@
       <c r="N30">
         <v>1</v>
       </c>
-      <c r="O30">
-        <v>1.5</v>
-      </c>
-      <c r="P30" t="b">
-        <v>1</v>
-      </c>
       <c r="Q30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2216,13 +2220,16 @@
       <c r="O31">
         <v>1</v>
       </c>
+      <c r="P31" t="b">
+        <v>1</v>
+      </c>
       <c r="Q31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -2264,15 +2271,15 @@
         <v>1</v>
       </c>
       <c r="O32">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="Q32" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -2316,31 +2323,137 @@
       <c r="O33">
         <v>1</v>
       </c>
+      <c r="P33" t="b">
+        <v>1</v>
+      </c>
       <c r="Q33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
       </c>
       <c r="Q34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35" t="b">
+        <v>1</v>
       </c>
       <c r="Q35" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>50</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="Q38" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mercenary update - added functionality to the mercenary dialog, not finished yet - added more images for panels and dialogs - made all area's movable dialogs with headers - added close and scrolling functionality for dialogs - added dragging for dialogs - misc other layout changes
</commit_message>
<xml_diff>
--- a/data/content/Stats.xlsx
+++ b/data/content/Stats.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\EndlessBattleFC\data\content\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="0" windowWidth="18000" windowHeight="18240"/>
+    <workbookView xWindow="12090" yWindow="0" windowWidth="18000" windowHeight="18240"/>
   </bookViews>
   <sheets>
     <sheet name="StatDefinition" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>name</t>
   </si>
@@ -295,6 +300,9 @@
   </si>
   <si>
     <t>MP/5 Multiplier: {0}%</t>
+  </si>
+  <si>
+    <t>valueMultiplier</t>
   </si>
 </sst>
 </file>
@@ -604,7 +612,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -612,13 +620,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R38"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K37" sqref="K37"/>
+      <selection pane="bottomRight" activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,11 +645,12 @@
     <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -691,13 +700,16 @@
         <v>47</v>
       </c>
       <c r="Q1" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" t="s">
         <v>87</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -743,11 +755,14 @@
       <c r="O2">
         <v>100</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2">
+        <v>1.01</v>
+      </c>
+      <c r="R2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -793,11 +808,14 @@
       <c r="O3">
         <v>100</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3">
+        <v>1.01</v>
+      </c>
+      <c r="R3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -846,11 +864,14 @@
       <c r="P4" t="b">
         <v>1</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -896,11 +917,14 @@
       <c r="O5">
         <v>5</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5">
+        <v>1.01</v>
+      </c>
+      <c r="R5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -949,11 +973,14 @@
       <c r="P6" t="b">
         <v>1</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -999,11 +1026,14 @@
       <c r="O7">
         <v>10</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7">
+        <v>1.01</v>
+      </c>
+      <c r="R7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1049,11 +1079,14 @@
       <c r="O8">
         <v>10</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8">
+        <v>1.01</v>
+      </c>
+      <c r="R8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1102,11 +1135,14 @@
       <c r="P9" t="b">
         <v>1</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -1152,11 +1188,14 @@
       <c r="O10">
         <v>5</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10">
+        <v>1.01</v>
+      </c>
+      <c r="R10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -1205,11 +1244,14 @@
       <c r="P11" t="b">
         <v>1</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1255,11 +1297,14 @@
       <c r="O12">
         <v>1</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q12">
+        <v>1.25</v>
+      </c>
+      <c r="R12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1305,11 +1350,14 @@
       <c r="O13">
         <v>1</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="Q13">
+        <v>1.25</v>
+      </c>
+      <c r="R13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1358,11 +1406,14 @@
       <c r="P14" t="b">
         <v>1</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Q14">
+        <v>1.3</v>
+      </c>
+      <c r="R14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1408,11 +1459,14 @@
       <c r="O15">
         <v>1</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="Q15">
+        <v>1.05</v>
+      </c>
+      <c r="R15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1461,11 +1515,14 @@
       <c r="P16" t="b">
         <v>1</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q16">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="R16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1511,11 +1568,14 @@
       <c r="O17">
         <v>1</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q17">
+        <v>1.05</v>
+      </c>
+      <c r="R17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1564,11 +1624,14 @@
       <c r="P18" t="b">
         <v>1</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="Q18">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="R18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1614,11 +1677,14 @@
       <c r="O19">
         <v>1</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="Q19">
+        <v>1.05</v>
+      </c>
+      <c r="R19" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1667,11 +1733,14 @@
       <c r="P20" t="b">
         <v>1</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="Q20">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="R20" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1717,11 +1786,14 @@
       <c r="O21">
         <v>1</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="Q21">
+        <v>1.05</v>
+      </c>
+      <c r="R21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1770,11 +1842,14 @@
       <c r="P22" t="b">
         <v>1</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="Q22">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="R22" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1817,11 +1892,14 @@
       <c r="N23">
         <v>1</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="Q23">
+        <v>1.01</v>
+      </c>
+      <c r="R23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1870,11 +1948,14 @@
       <c r="P24" t="b">
         <v>1</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="Q24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1917,11 +1998,14 @@
       <c r="N25">
         <v>1</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="Q25">
+        <v>1.02</v>
+      </c>
+      <c r="R25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1970,11 +2054,14 @@
       <c r="P26" t="b">
         <v>1</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="Q26">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="R26" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2017,11 +2104,14 @@
       <c r="N27">
         <v>1</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="Q27">
+        <v>1.2</v>
+      </c>
+      <c r="R27" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -2070,11 +2160,14 @@
       <c r="P28" t="b">
         <v>1</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="Q28">
+        <v>1.2</v>
+      </c>
+      <c r="R28" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -2123,11 +2216,14 @@
       <c r="P29" t="b">
         <v>1</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="Q29">
+        <v>1.3</v>
+      </c>
+      <c r="R29" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -2170,11 +2266,14 @@
       <c r="N30">
         <v>1</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="Q30">
+        <v>1.02</v>
+      </c>
+      <c r="R30" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -2223,11 +2322,14 @@
       <c r="P31" t="b">
         <v>1</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="Q31">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="R31" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -2273,11 +2375,14 @@
       <c r="O32">
         <v>1.5</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="Q32">
+        <v>1.02</v>
+      </c>
+      <c r="R32" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -2326,11 +2431,14 @@
       <c r="P33" t="b">
         <v>1</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="Q33">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="R33" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -2376,11 +2484,14 @@
       <c r="O34">
         <v>1</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="Q34">
+        <v>1.05</v>
+      </c>
+      <c r="R34" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -2429,31 +2540,34 @@
       <c r="P35" t="b">
         <v>1</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="Q35">
+        <v>1.2</v>
+      </c>
+      <c r="R35" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>48</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="R36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>49</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="R37" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>50</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="R38" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Player XP Fix - fixed the player xp temporarily when loading data - added two mercenary related stats - added most of the ui images into the source folder - updated jquery and jquery ui references to latest stable - removed no longer needed images
</commit_message>
<xml_diff>
--- a/data/content/Stats.xlsx
+++ b/data/content/Stats.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12090" yWindow="0" windowWidth="18000" windowHeight="18240"/>
+    <workbookView xWindow="13020" yWindow="0" windowWidth="18000" windowHeight="18240"/>
   </bookViews>
   <sheets>
     <sheet name="StatDefinition" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>name</t>
   </si>
@@ -303,6 +303,18 @@
   </si>
   <si>
     <t>valueMultiplier</t>
+  </si>
+  <si>
+    <t>mercGpsMult</t>
+  </si>
+  <si>
+    <t>mercCostMult</t>
+  </si>
+  <si>
+    <t>Mercenary Cost Reduction: {0}</t>
+  </si>
+  <si>
+    <t>Mercenary GPS Multiplier: {0}</t>
   </si>
 </sst>
 </file>
@@ -620,13 +632,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S38"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q36" sqref="Q36"/>
+      <selection pane="bottomRight" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2549,25 +2561,137 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>94</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <v>1.1000000000000001</v>
       </c>
       <c r="R36" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>93</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>1</v>
+      </c>
+      <c r="P37" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q37">
+        <v>1.1000000000000001</v>
       </c>
       <c r="R37" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="R38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+      <c r="R39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>50</v>
       </c>
-      <c r="R38" t="s">
+      <c r="R40" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Item data - small update to stats table to be consistent with new item data file
</commit_message>
<xml_diff>
--- a/data/content/Stats.xlsx
+++ b/data/content/Stats.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="0" windowWidth="18000" windowHeight="18240"/>
+    <workbookView xWindow="13950" yWindow="0" windowWidth="18000" windowHeight="18240"/>
   </bookViews>
   <sheets>
     <sheet name="StatDefinition" sheetId="1" r:id="rId1"/>
@@ -128,9 +128,6 @@
     <t>ringMult</t>
   </si>
   <si>
-    <t>amuletMult</t>
-  </si>
-  <si>
     <t>magicFind</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>Mercenary GPS Multiplier: {0}</t>
+  </si>
+  <si>
+    <t>neckMult</t>
   </si>
 </sst>
 </file>
@@ -635,10 +635,10 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J42" sqref="J42"/>
+      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,22 +703,22 @@
         <v>33</v>
       </c>
       <c r="N1" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="O1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -771,7 +771,7 @@
         <v>1.01</v>
       </c>
       <c r="R2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -824,7 +824,7 @@
         <v>1.01</v>
       </c>
       <c r="R3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -880,7 +880,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="R4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -933,7 +933,7 @@
         <v>1.01</v>
       </c>
       <c r="R5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -989,7 +989,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="R6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1042,7 +1042,7 @@
         <v>1.01</v>
       </c>
       <c r="R7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1095,7 +1095,7 @@
         <v>1.01</v>
       </c>
       <c r="R8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1151,12 +1151,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="R9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1204,12 +1204,12 @@
         <v>1.01</v>
       </c>
       <c r="R10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1260,7 +1260,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="R11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1313,7 +1313,7 @@
         <v>1.25</v>
       </c>
       <c r="R12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1366,7 +1366,7 @@
         <v>1.25</v>
       </c>
       <c r="R13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1422,7 +1422,7 @@
         <v>1.3</v>
       </c>
       <c r="R14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1475,7 +1475,7 @@
         <v>1.05</v>
       </c>
       <c r="R15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1531,7 +1531,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="R16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -1584,7 +1584,7 @@
         <v>1.05</v>
       </c>
       <c r="R17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -1640,7 +1640,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="R18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -1693,7 +1693,7 @@
         <v>1.05</v>
       </c>
       <c r="R19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -1749,7 +1749,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="R20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -1802,7 +1802,7 @@
         <v>1.05</v>
       </c>
       <c r="R21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -1858,7 +1858,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="R22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -1908,7 +1908,7 @@
         <v>1.01</v>
       </c>
       <c r="R23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -1964,12 +1964,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="R24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2014,12 +2014,12 @@
         <v>1.02</v>
       </c>
       <c r="R25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2070,12 +2070,12 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="R26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2120,12 +2120,12 @@
         <v>1.2</v>
       </c>
       <c r="R27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2176,12 +2176,12 @@
         <v>1.2</v>
       </c>
       <c r="R28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2232,12 +2232,12 @@
         <v>1.3</v>
       </c>
       <c r="R29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -2282,12 +2282,12 @@
         <v>1.02</v>
       </c>
       <c r="R30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2338,12 +2338,12 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="R31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -2391,12 +2391,12 @@
         <v>1.02</v>
       </c>
       <c r="R32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -2447,12 +2447,12 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="R33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -2500,12 +2500,12 @@
         <v>1.05</v>
       </c>
       <c r="R34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -2556,12 +2556,12 @@
         <v>1.2</v>
       </c>
       <c r="R35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -2612,12 +2612,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="R36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -2668,31 +2668,31 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="R37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monster Generation - added first pass on updated monster generation using the data driven stats and templates - updated CrystalBuild binaries to latest version - made UIElement a little less verbose by default - updates to stat definitions and monster data
</commit_message>
<xml_diff>
--- a/data/content/Stats.xlsx
+++ b/data/content/Stats.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\EndlessBattleFC\data\content\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="13950" yWindow="0" windowWidth="18000" windowHeight="18240"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>name</t>
   </si>
@@ -315,6 +310,27 @@
   </si>
   <si>
     <t>neckMult</t>
+  </si>
+  <si>
+    <t>statMult</t>
+  </si>
+  <si>
+    <t>Stat Multiplier: {0}</t>
+  </si>
+  <si>
+    <t>rarity</t>
+  </si>
+  <si>
+    <t>Rarity: {0}</t>
+  </si>
+  <si>
+    <t>isSecondaryStat</t>
+  </si>
+  <si>
+    <t>isPrimaryStat</t>
+  </si>
+  <si>
+    <t>isTertiaryStat</t>
   </si>
 </sst>
 </file>
@@ -624,7 +640,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -632,13 +648,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,12 +673,15 @@
     <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -712,16 +731,25 @@
         <v>46</v>
       </c>
       <c r="Q1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R1" t="s">
+        <v>101</v>
+      </c>
+      <c r="S1" t="s">
+        <v>103</v>
+      </c>
+      <c r="T1" t="s">
         <v>91</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>86</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -767,14 +795,14 @@
       <c r="O2">
         <v>100</v>
       </c>
-      <c r="Q2">
+      <c r="T2">
         <v>1.01</v>
       </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -820,14 +848,17 @@
       <c r="O3">
         <v>100</v>
       </c>
-      <c r="Q3">
+      <c r="R3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3">
         <v>1.01</v>
       </c>
-      <c r="R3" t="s">
+      <c r="U3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -876,14 +907,17 @@
       <c r="P4" t="b">
         <v>1</v>
       </c>
-      <c r="Q4">
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="R4" t="s">
+      <c r="U4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -929,14 +963,17 @@
       <c r="O5">
         <v>5</v>
       </c>
-      <c r="Q5">
+      <c r="R5" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5">
         <v>1.01</v>
       </c>
-      <c r="R5" t="s">
+      <c r="U5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -985,14 +1022,17 @@
       <c r="P6" t="b">
         <v>1</v>
       </c>
-      <c r="Q6">
+      <c r="R6" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="R6" t="s">
+      <c r="U6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1038,14 +1078,14 @@
       <c r="O7">
         <v>10</v>
       </c>
-      <c r="Q7">
+      <c r="T7">
         <v>1.01</v>
       </c>
-      <c r="R7" t="s">
+      <c r="U7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1091,14 +1131,17 @@
       <c r="O8">
         <v>10</v>
       </c>
-      <c r="Q8">
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8">
         <v>1.01</v>
       </c>
-      <c r="R8" t="s">
+      <c r="U8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1147,14 +1190,17 @@
       <c r="P9" t="b">
         <v>1</v>
       </c>
-      <c r="Q9">
+      <c r="R9" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="R9" t="s">
+      <c r="U9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -1200,14 +1246,17 @@
       <c r="O10">
         <v>5</v>
       </c>
-      <c r="Q10">
+      <c r="R10" t="b">
+        <v>1</v>
+      </c>
+      <c r="T10">
         <v>1.01</v>
       </c>
-      <c r="R10" t="s">
+      <c r="U10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -1256,14 +1305,17 @@
       <c r="P11" t="b">
         <v>1</v>
       </c>
-      <c r="Q11">
+      <c r="R11" t="b">
+        <v>1</v>
+      </c>
+      <c r="T11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="R11" t="s">
+      <c r="U11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1309,14 +1361,17 @@
       <c r="O12">
         <v>1</v>
       </c>
-      <c r="Q12">
+      <c r="R12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T12">
         <v>1.25</v>
       </c>
-      <c r="R12" t="s">
+      <c r="U12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1362,14 +1417,17 @@
       <c r="O13">
         <v>1</v>
       </c>
-      <c r="Q13">
+      <c r="R13" t="b">
+        <v>1</v>
+      </c>
+      <c r="T13">
         <v>1.25</v>
       </c>
-      <c r="R13" t="s">
+      <c r="U13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1418,14 +1476,17 @@
       <c r="P14" t="b">
         <v>1</v>
       </c>
-      <c r="Q14">
+      <c r="R14" t="b">
+        <v>1</v>
+      </c>
+      <c r="T14">
         <v>1.3</v>
       </c>
-      <c r="R14" t="s">
+      <c r="U14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1471,14 +1532,17 @@
       <c r="O15">
         <v>1</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" t="b">
+        <v>1</v>
+      </c>
+      <c r="T15">
         <v>1.05</v>
       </c>
-      <c r="R15" t="s">
+      <c r="U15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1527,14 +1591,17 @@
       <c r="P16" t="b">
         <v>1</v>
       </c>
-      <c r="Q16">
+      <c r="R16" t="b">
+        <v>1</v>
+      </c>
+      <c r="T16">
         <v>1.1499999999999999</v>
       </c>
-      <c r="R16" t="s">
+      <c r="U16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1580,14 +1647,17 @@
       <c r="O17">
         <v>1</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" t="b">
+        <v>1</v>
+      </c>
+      <c r="T17">
         <v>1.05</v>
       </c>
-      <c r="R17" t="s">
+      <c r="U17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1636,14 +1706,17 @@
       <c r="P18" t="b">
         <v>1</v>
       </c>
-      <c r="Q18">
+      <c r="R18" t="b">
+        <v>1</v>
+      </c>
+      <c r="T18">
         <v>1.1499999999999999</v>
       </c>
-      <c r="R18" t="s">
+      <c r="U18" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1689,14 +1762,17 @@
       <c r="O19">
         <v>1</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" t="b">
+        <v>1</v>
+      </c>
+      <c r="T19">
         <v>1.05</v>
       </c>
-      <c r="R19" t="s">
+      <c r="U19" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1745,14 +1821,17 @@
       <c r="P20" t="b">
         <v>1</v>
       </c>
-      <c r="Q20">
+      <c r="R20" t="b">
+        <v>1</v>
+      </c>
+      <c r="T20">
         <v>1.1499999999999999</v>
       </c>
-      <c r="R20" t="s">
+      <c r="U20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1798,14 +1877,17 @@
       <c r="O21">
         <v>1</v>
       </c>
-      <c r="Q21">
+      <c r="R21" t="b">
+        <v>1</v>
+      </c>
+      <c r="T21">
         <v>1.05</v>
       </c>
-      <c r="R21" t="s">
+      <c r="U21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1854,14 +1936,17 @@
       <c r="P22" t="b">
         <v>1</v>
       </c>
-      <c r="Q22">
+      <c r="R22" t="b">
+        <v>1</v>
+      </c>
+      <c r="T22">
         <v>1.1499999999999999</v>
       </c>
-      <c r="R22" t="s">
+      <c r="U22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1904,14 +1989,17 @@
       <c r="N23">
         <v>1</v>
       </c>
-      <c r="Q23">
+      <c r="R23" t="b">
+        <v>1</v>
+      </c>
+      <c r="T23">
         <v>1.01</v>
       </c>
-      <c r="R23" t="s">
+      <c r="U23" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1960,14 +2048,17 @@
       <c r="P24" t="b">
         <v>1</v>
       </c>
-      <c r="Q24">
+      <c r="R24" t="b">
+        <v>1</v>
+      </c>
+      <c r="T24">
         <v>1.1000000000000001</v>
       </c>
-      <c r="R24" t="s">
+      <c r="U24" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -2010,14 +2101,17 @@
       <c r="N25">
         <v>1</v>
       </c>
-      <c r="Q25">
+      <c r="R25" t="b">
+        <v>1</v>
+      </c>
+      <c r="T25">
         <v>1.02</v>
       </c>
-      <c r="R25" t="s">
+      <c r="U25" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -2066,14 +2160,17 @@
       <c r="P26" t="b">
         <v>1</v>
       </c>
-      <c r="Q26">
+      <c r="R26" t="b">
+        <v>1</v>
+      </c>
+      <c r="T26">
         <v>1.1100000000000001</v>
       </c>
-      <c r="R26" t="s">
+      <c r="U26" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2116,14 +2213,17 @@
       <c r="N27">
         <v>1</v>
       </c>
-      <c r="Q27">
+      <c r="S27" t="b">
+        <v>1</v>
+      </c>
+      <c r="T27">
         <v>1.2</v>
       </c>
-      <c r="R27" t="s">
+      <c r="U27" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -2172,14 +2272,17 @@
       <c r="P28" t="b">
         <v>1</v>
       </c>
-      <c r="Q28">
+      <c r="S28" t="b">
+        <v>1</v>
+      </c>
+      <c r="T28">
         <v>1.2</v>
       </c>
-      <c r="R28" t="s">
+      <c r="U28" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2228,14 +2331,17 @@
       <c r="P29" t="b">
         <v>1</v>
       </c>
-      <c r="Q29">
+      <c r="S29" t="b">
+        <v>1</v>
+      </c>
+      <c r="T29">
         <v>1.3</v>
       </c>
-      <c r="R29" t="s">
+      <c r="U29" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -2278,14 +2384,17 @@
       <c r="N30">
         <v>1</v>
       </c>
-      <c r="Q30">
+      <c r="R30" t="b">
+        <v>1</v>
+      </c>
+      <c r="T30">
         <v>1.02</v>
       </c>
-      <c r="R30" t="s">
+      <c r="U30" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -2334,14 +2443,17 @@
       <c r="P31" t="b">
         <v>1</v>
       </c>
-      <c r="Q31">
+      <c r="R31" t="b">
+        <v>1</v>
+      </c>
+      <c r="T31">
         <v>1.1100000000000001</v>
       </c>
-      <c r="R31" t="s">
+      <c r="U31" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -2387,14 +2499,20 @@
       <c r="O32">
         <v>1.5</v>
       </c>
-      <c r="Q32">
+      <c r="P32" t="b">
+        <v>1</v>
+      </c>
+      <c r="R32" t="b">
+        <v>1</v>
+      </c>
+      <c r="T32">
         <v>1.02</v>
       </c>
-      <c r="R32" t="s">
+      <c r="U32" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -2443,14 +2561,17 @@
       <c r="P33" t="b">
         <v>1</v>
       </c>
-      <c r="Q33">
+      <c r="R33" t="b">
+        <v>1</v>
+      </c>
+      <c r="T33">
         <v>1.1100000000000001</v>
       </c>
-      <c r="R33" t="s">
+      <c r="U33" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -2496,14 +2617,20 @@
       <c r="O34">
         <v>1</v>
       </c>
-      <c r="Q34">
+      <c r="P34" t="b">
+        <v>1</v>
+      </c>
+      <c r="R34" t="b">
+        <v>1</v>
+      </c>
+      <c r="T34">
         <v>1.05</v>
       </c>
-      <c r="R34" t="s">
+      <c r="U34" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -2552,14 +2679,17 @@
       <c r="P35" t="b">
         <v>1</v>
       </c>
-      <c r="Q35">
+      <c r="R35" t="b">
+        <v>1</v>
+      </c>
+      <c r="T35">
         <v>1.2</v>
       </c>
-      <c r="R35" t="s">
+      <c r="U35" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -2608,14 +2738,17 @@
       <c r="P36" t="b">
         <v>1</v>
       </c>
-      <c r="Q36">
+      <c r="S36" t="b">
+        <v>1</v>
+      </c>
+      <c r="T36">
         <v>1.1000000000000001</v>
       </c>
-      <c r="R36" t="s">
+      <c r="U36" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>92</v>
       </c>
@@ -2664,35 +2797,63 @@
       <c r="P37" t="b">
         <v>1</v>
       </c>
-      <c r="Q37">
+      <c r="S37" t="b">
+        <v>1</v>
+      </c>
+      <c r="T37">
         <v>1.1000000000000001</v>
       </c>
-      <c r="R37" t="s">
+      <c r="U37" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>97</v>
+      </c>
+      <c r="O38">
+        <v>1</v>
+      </c>
+      <c r="P38" t="b">
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <v>1.4</v>
+      </c>
+      <c r="U38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>47</v>
       </c>
-      <c r="R38" t="s">
+      <c r="U39" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>48</v>
       </c>
-      <c r="R39" t="s">
+      <c r="U40" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>49</v>
       </c>
-      <c r="R40" t="s">
+      <c r="U41" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>99</v>
+      </c>
+      <c r="U42" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monster generation - some fixes to monster generation, basic stats are now working as intended - small fix to inventory
</commit_message>
<xml_diff>
--- a/data/content/Stats.xlsx
+++ b/data/content/Stats.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\EndlessBattleFC\data\content\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13950" yWindow="0" windowWidth="18000" windowHeight="18240"/>
+    <workbookView xWindow="14880" yWindow="0" windowWidth="18000" windowHeight="18240"/>
   </bookViews>
   <sheets>
     <sheet name="StatDefinition" sheetId="1" r:id="rId1"/>
@@ -640,7 +645,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -654,7 +659,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
+      <selection pane="bottomRight" activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Combat update - Monsters now get a type generated - Display and combat now uses the new actor monster - Basic combat is working but missing rewards and ability cycles - trimmed the resistances a little - raised min hit chance to 50% - fixed infinite resurrection loop
</commit_message>
<xml_diff>
--- a/data/content/Stats.xlsx
+++ b/data/content/Stats.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15810" yWindow="0" windowWidth="18000" windowHeight="18240"/>
+    <workbookView xWindow="17670" yWindow="0" windowWidth="18000" windowHeight="18240"/>
   </bookViews>
   <sheets>
     <sheet name="StatDefinition" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>name</t>
   </si>
@@ -353,33 +353,21 @@
     <t>fireDmgMult</t>
   </si>
   <si>
-    <t>coldDmgMult</t>
-  </si>
-  <si>
     <t>lightDmgMult</t>
   </si>
   <si>
     <t>darkDmgMult</t>
   </si>
   <si>
-    <t>holyDmgMult</t>
-  </si>
-  <si>
     <t>fireResist</t>
   </si>
   <si>
-    <t>coldResist</t>
-  </si>
-  <si>
     <t>lightResist</t>
   </si>
   <si>
     <t>fireResistMult</t>
   </si>
   <si>
-    <t>coldResistMult</t>
-  </si>
-  <si>
     <t>lightResistMult</t>
   </si>
   <si>
@@ -389,12 +377,6 @@
     <t>darkResistMult</t>
   </si>
   <si>
-    <t>holyResist</t>
-  </si>
-  <si>
-    <t>holyResistMult</t>
-  </si>
-  <si>
     <t>resistAll</t>
   </si>
   <si>
@@ -404,63 +386,36 @@
     <t>fireDmgConv</t>
   </si>
   <si>
-    <t>coldDmgConv</t>
-  </si>
-  <si>
     <t>lightDmgConv</t>
   </si>
   <si>
     <t>darkDmgConv</t>
   </si>
   <si>
-    <t>holyDmgConv</t>
-  </si>
-  <si>
     <t>Fire Dmg Multiplier: {0}</t>
   </si>
   <si>
-    <t>Cold Dmg Multiplier: {0}</t>
-  </si>
-  <si>
     <t>Dark Dmg Multiplier: {0}</t>
   </si>
   <si>
-    <t>Holy Dmg Multiplier: {0}</t>
-  </si>
-  <si>
     <t>Fire Resist Multiplier: {0}</t>
   </si>
   <si>
-    <t>Cold Resist Multiplier: {0}</t>
-  </si>
-  <si>
     <t>Dark Resist Multiplier: {0}</t>
   </si>
   <si>
-    <t>Holy Resist Multiplier: {0}</t>
-  </si>
-  <si>
     <t>Resist All Multiplier: {0}</t>
   </si>
   <si>
     <t>Lightning Dmg Multiplier: {0}</t>
   </si>
   <si>
-    <t>Lightning Resist Multiplier: {0}</t>
-  </si>
-  <si>
     <t>{0}% of dmg as Fire</t>
   </si>
   <si>
-    <t>{0}% of dmg as Cold</t>
-  </si>
-  <si>
     <t>{0}% of dmg as Dark</t>
   </si>
   <si>
-    <t>{0}% of dmg as Holy</t>
-  </si>
-  <si>
     <t>{0}% of dmg as Lightning</t>
   </si>
   <si>
@@ -470,16 +425,37 @@
     <t>Resist All: {0}</t>
   </si>
   <si>
-    <t>Cold Resist: {0}</t>
-  </si>
-  <si>
-    <t>Lightning Resist: {0}</t>
-  </si>
-  <si>
     <t>Dark Resist: {0}</t>
   </si>
   <si>
-    <t>Holy Resist: {0}</t>
+    <t>Light resist: {0}</t>
+  </si>
+  <si>
+    <t>Light Resist Multiplier: {0}</t>
+  </si>
+  <si>
+    <t>Ice Resist: {0}</t>
+  </si>
+  <si>
+    <t>Ice Resist Multiplier: {0}</t>
+  </si>
+  <si>
+    <t>iceResist</t>
+  </si>
+  <si>
+    <t>iceResistMult</t>
+  </si>
+  <si>
+    <t>iceDmgMult</t>
+  </si>
+  <si>
+    <t>iceDmgConv</t>
+  </si>
+  <si>
+    <t>{0}% of dmg as Ice</t>
+  </si>
+  <si>
+    <t>Ice Dmg Multiplier: {0}</t>
   </si>
 </sst>
 </file>
@@ -797,13 +773,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V66"/>
+  <dimension ref="A1:V62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N63" sqref="N63"/>
+      <selection pane="bottomRight" activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3097,12 +3073,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U40" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -3153,12 +3129,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U41" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -3209,12 +3185,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U42" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -3265,12 +3241,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U43" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -3317,16 +3293,19 @@
       <c r="P44" t="b">
         <v>1</v>
       </c>
+      <c r="R44" t="b">
+        <v>1</v>
+      </c>
       <c r="T44">
-        <v>1.1000000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="U44" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -3380,12 +3359,12 @@
         <v>1.05</v>
       </c>
       <c r="U45" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -3439,12 +3418,12 @@
         <v>1.05</v>
       </c>
       <c r="U46" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -3498,12 +3477,12 @@
         <v>1.05</v>
       </c>
       <c r="U47" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -3545,9 +3524,6 @@
         <v>1</v>
       </c>
       <c r="O48">
-        <v>1</v>
-      </c>
-      <c r="P48" t="b">
         <v>1</v>
       </c>
       <c r="R48" t="b">
@@ -3557,12 +3533,12 @@
         <v>1.05</v>
       </c>
       <c r="U48" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -3609,19 +3585,16 @@
       <c r="P49" t="b">
         <v>1</v>
       </c>
-      <c r="R49" t="b">
-        <v>1</v>
-      </c>
       <c r="T49">
-        <v>1.05</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="U49" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -3672,12 +3645,12 @@
         <v>1.05</v>
       </c>
       <c r="U50" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -3728,12 +3701,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U51" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -3784,12 +3757,12 @@
         <v>1.05</v>
       </c>
       <c r="U52" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -3896,12 +3869,12 @@
         <v>1.05</v>
       </c>
       <c r="U54" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -3952,12 +3925,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U55" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -4005,296 +3978,72 @@
         <v>1</v>
       </c>
       <c r="T56">
-        <v>1.05</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="U56" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>120</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-      <c r="F57">
-        <v>1</v>
-      </c>
-      <c r="G57">
-        <v>1</v>
-      </c>
-      <c r="H57">
-        <v>1</v>
-      </c>
-      <c r="I57">
-        <v>1</v>
-      </c>
-      <c r="J57">
-        <v>1</v>
-      </c>
-      <c r="K57">
-        <v>1</v>
-      </c>
-      <c r="L57">
-        <v>1</v>
-      </c>
-      <c r="M57">
-        <v>1</v>
-      </c>
-      <c r="N57">
-        <v>1</v>
-      </c>
-      <c r="O57">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="P57" t="b">
         <v>1</v>
       </c>
       <c r="T57">
-        <v>1.1000000000000001</v>
+        <v>1.25</v>
       </c>
       <c r="U57" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>121</v>
-      </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-      <c r="F58">
-        <v>1</v>
-      </c>
-      <c r="G58">
-        <v>1</v>
-      </c>
-      <c r="H58">
-        <v>1</v>
-      </c>
-      <c r="I58">
-        <v>1</v>
-      </c>
-      <c r="J58">
-        <v>1</v>
-      </c>
-      <c r="K58">
-        <v>1</v>
-      </c>
-      <c r="L58">
-        <v>1</v>
-      </c>
-      <c r="M58">
-        <v>1</v>
-      </c>
-      <c r="N58">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="O58">
         <v>1</v>
       </c>
-      <c r="R58" t="b">
+      <c r="P58" t="b">
         <v>1</v>
       </c>
       <c r="T58">
-        <v>1.05</v>
+        <v>1.4</v>
       </c>
       <c r="U58" t="s">
-        <v>151</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>122</v>
-      </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59">
-        <v>1</v>
-      </c>
-      <c r="F59">
-        <v>1</v>
-      </c>
-      <c r="G59">
-        <v>1</v>
-      </c>
-      <c r="H59">
-        <v>1</v>
-      </c>
-      <c r="I59">
-        <v>1</v>
-      </c>
-      <c r="J59">
-        <v>1</v>
-      </c>
-      <c r="K59">
-        <v>1</v>
-      </c>
-      <c r="L59">
-        <v>1</v>
-      </c>
-      <c r="M59">
-        <v>1</v>
-      </c>
-      <c r="N59">
-        <v>1</v>
-      </c>
-      <c r="O59">
-        <v>1</v>
-      </c>
-      <c r="P59" t="b">
-        <v>1</v>
-      </c>
-      <c r="T59">
-        <v>1.1000000000000001</v>
+        <v>47</v>
       </c>
       <c r="U59" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>123</v>
-      </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-      <c r="F60">
-        <v>1</v>
-      </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
-      <c r="H60">
-        <v>1</v>
-      </c>
-      <c r="I60">
-        <v>1</v>
-      </c>
-      <c r="J60">
-        <v>1</v>
-      </c>
-      <c r="K60">
-        <v>1</v>
-      </c>
-      <c r="L60">
-        <v>1</v>
-      </c>
-      <c r="M60">
-        <v>1</v>
-      </c>
-      <c r="N60">
-        <v>1</v>
-      </c>
-      <c r="O60">
-        <v>1</v>
-      </c>
-      <c r="R60" t="b">
-        <v>1</v>
-      </c>
-      <c r="T60">
-        <v>1.1499999999999999</v>
+        <v>48</v>
       </c>
       <c r="U60" t="s">
-        <v>147</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>124</v>
-      </c>
-      <c r="P61" t="b">
-        <v>1</v>
-      </c>
-      <c r="T61">
-        <v>1.25</v>
+        <v>49</v>
       </c>
       <c r="U61" t="s">
-        <v>138</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>97</v>
-      </c>
-      <c r="O62">
-        <v>1</v>
-      </c>
-      <c r="P62" t="b">
-        <v>1</v>
-      </c>
-      <c r="T62">
-        <v>1.4</v>
+        <v>99</v>
       </c>
       <c r="U62" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>47</v>
-      </c>
-      <c r="U63" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>48</v>
-      </c>
-      <c r="U64" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>49</v>
-      </c>
-      <c r="U65" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>99</v>
-      </c>
-      <c r="U66" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Character Stat display - stats for player are now displayed in categorized list
</commit_message>
<xml_diff>
--- a/data/content/Stats.xlsx
+++ b/data/content/Stats.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17670" yWindow="0" windowWidth="18000" windowHeight="18240"/>
+    <workbookView xWindow="24180" yWindow="0" windowWidth="18000" windowHeight="18240"/>
   </bookViews>
   <sheets>
     <sheet name="StatDefinition" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="148">
   <si>
     <t>name</t>
   </si>
@@ -179,126 +179,12 @@
     <t>tooltip</t>
   </si>
   <si>
-    <t>HP/5: {0}</t>
-  </si>
-  <si>
-    <t>HP: {0}</t>
-  </si>
-  <si>
-    <t>MP: {0}</t>
-  </si>
-  <si>
-    <t>XP: {0}</t>
-  </si>
-  <si>
-    <t>HP Multiplier: {0}%</t>
-  </si>
-  <si>
-    <t>MP Multiplier: {0}%</t>
-  </si>
-  <si>
-    <t>HP/5 Multiplier: {0}%</t>
-  </si>
-  <si>
-    <t>MP Max: {0}</t>
-  </si>
-  <si>
-    <t>HP Max: {0}</t>
-  </si>
-  <si>
-    <t>Min Damage: {0}</t>
-  </si>
-  <si>
-    <t>Max Damage: {0}</t>
-  </si>
-  <si>
-    <t>Damage Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Strength: {0}</t>
-  </si>
-  <si>
-    <t>Strength Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Agility: {0}</t>
-  </si>
-  <si>
-    <t>Agility Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Intelligence: {0}</t>
-  </si>
-  <si>
-    <t>Intelligence Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Stamina: {0}</t>
-  </si>
-  <si>
-    <t>Stamina Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Armor: {0}</t>
-  </si>
-  <si>
-    <t>Armor Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Evasion Rating: {0}</t>
-  </si>
-  <si>
-    <t>Evasion Rating Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Magic find: {0}</t>
-  </si>
-  <si>
-    <t>Gold Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>XP Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Crit Rating: {0}</t>
-  </si>
-  <si>
-    <t>Crit Damage: {0}</t>
-  </si>
-  <si>
-    <t>Crit Rating Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Crit Damage Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Speed: {0}</t>
-  </si>
-  <si>
-    <t>Speed Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Gold: {0}</t>
-  </si>
-  <si>
-    <t>Shards: {0}</t>
-  </si>
-  <si>
-    <t>displayString</t>
-  </si>
-  <si>
     <t>mp5</t>
   </si>
   <si>
     <t>mp5Mult</t>
   </si>
   <si>
-    <t>MP/5: {0}</t>
-  </si>
-  <si>
-    <t>MP/5 Multiplier: {0}%</t>
-  </si>
-  <si>
     <t>valueMultiplier</t>
   </si>
   <si>
@@ -308,27 +194,15 @@
     <t>mercCostMult</t>
   </si>
   <si>
-    <t>Mercenary Cost Reduction: {0}</t>
-  </si>
-  <si>
-    <t>Mercenary GPS Multiplier: {0}</t>
-  </si>
-  <si>
     <t>neckMult</t>
   </si>
   <si>
     <t>statMult</t>
   </si>
   <si>
-    <t>Stat Multiplier: {0}</t>
-  </si>
-  <si>
     <t>rarity</t>
   </si>
   <si>
-    <t>Rarity: {0}</t>
-  </si>
-  <si>
     <t>isSecondaryStat</t>
   </si>
   <si>
@@ -344,12 +218,6 @@
     <t>hitRateMult</t>
   </si>
   <si>
-    <t>Hit Rate: {0}</t>
-  </si>
-  <si>
-    <t>Hit Rate Multiplier: {0}</t>
-  </si>
-  <si>
     <t>fireDmgMult</t>
   </si>
   <si>
@@ -392,54 +260,6 @@
     <t>darkDmgConv</t>
   </si>
   <si>
-    <t>Fire Dmg Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Dark Dmg Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Fire Resist Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Dark Resist Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Resist All Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Lightning Dmg Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>{0}% of dmg as Fire</t>
-  </si>
-  <si>
-    <t>{0}% of dmg as Dark</t>
-  </si>
-  <si>
-    <t>{0}% of dmg as Lightning</t>
-  </si>
-  <si>
-    <t>Fire Resist: {0}</t>
-  </si>
-  <si>
-    <t>Resist All: {0}</t>
-  </si>
-  <si>
-    <t>Dark Resist: {0}</t>
-  </si>
-  <si>
-    <t>Light resist: {0}</t>
-  </si>
-  <si>
-    <t>Light Resist Multiplier: {0}</t>
-  </si>
-  <si>
-    <t>Ice Resist: {0}</t>
-  </si>
-  <si>
-    <t>Ice Resist Multiplier: {0}</t>
-  </si>
-  <si>
     <t>iceResist</t>
   </si>
   <si>
@@ -452,10 +272,202 @@
     <t>iceDmgConv</t>
   </si>
   <si>
-    <t>{0}% of dmg as Ice</t>
-  </si>
-  <si>
-    <t>Ice Dmg Multiplier: {0}</t>
+    <t>displayCategory</t>
+  </si>
+  <si>
+    <t>Base Stats</t>
+  </si>
+  <si>
+    <t>Defensive</t>
+  </si>
+  <si>
+    <t>Offensive</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>displayValue</t>
+  </si>
+  <si>
+    <t>displayHeader</t>
+  </si>
+  <si>
+    <t>{0}</t>
+  </si>
+  <si>
+    <t>{0}%</t>
+  </si>
+  <si>
+    <t>{0}/5</t>
+  </si>
+  <si>
+    <t>Strength Multiplier</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>HP Multiplier</t>
+  </si>
+  <si>
+    <t>HP/5</t>
+  </si>
+  <si>
+    <t>HP/5 Multiplier</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>MP Multiplier</t>
+  </si>
+  <si>
+    <t>MP/5</t>
+  </si>
+  <si>
+    <t>MP/5 Multiplier</t>
+  </si>
+  <si>
+    <t>Min Damage</t>
+  </si>
+  <si>
+    <t>Max Damage</t>
+  </si>
+  <si>
+    <t>Damage Multiplier</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Agility</t>
+  </si>
+  <si>
+    <t>Agility Multiplier</t>
+  </si>
+  <si>
+    <t>Intelligence</t>
+  </si>
+  <si>
+    <t>Intelligence Multiplier</t>
+  </si>
+  <si>
+    <t>Stamina</t>
+  </si>
+  <si>
+    <t>Stamina Multiplier</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Armor Multiplier</t>
+  </si>
+  <si>
+    <t>Evasion Rating</t>
+  </si>
+  <si>
+    <t>Evasion Rating Multiplier</t>
+  </si>
+  <si>
+    <t>Magic find</t>
+  </si>
+  <si>
+    <t>Gold Multiplier</t>
+  </si>
+  <si>
+    <t>XP Multiplier</t>
+  </si>
+  <si>
+    <t>Crit Rating</t>
+  </si>
+  <si>
+    <t>Crit Rating Multiplier</t>
+  </si>
+  <si>
+    <t>Crit Damage</t>
+  </si>
+  <si>
+    <t>Crit Damage Multiplier</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Speed Multiplier</t>
+  </si>
+  <si>
+    <t>Mercenary Cost Reduction</t>
+  </si>
+  <si>
+    <t>Mercenary GPS Multiplier</t>
+  </si>
+  <si>
+    <t>Hit Rate</t>
+  </si>
+  <si>
+    <t>Hit Rate Multiplier</t>
+  </si>
+  <si>
+    <t>Fire Dmg Multiplier</t>
+  </si>
+  <si>
+    <t>Ice Dmg Multiplier</t>
+  </si>
+  <si>
+    <t>Lightning Dmg Multiplier</t>
+  </si>
+  <si>
+    <t>Dark Dmg Multiplier</t>
+  </si>
+  <si>
+    <t>Damage as Fire</t>
+  </si>
+  <si>
+    <t>Damage as Ice</t>
+  </si>
+  <si>
+    <t>Damage as Light</t>
+  </si>
+  <si>
+    <t>Damage as Dark</t>
+  </si>
+  <si>
+    <t>Fire Resist</t>
+  </si>
+  <si>
+    <t>Fire Resist Multiplier</t>
+  </si>
+  <si>
+    <t>Ice Resist</t>
+  </si>
+  <si>
+    <t>Ice Resist Multiplier</t>
+  </si>
+  <si>
+    <t>Light resist</t>
+  </si>
+  <si>
+    <t>Light Resist Multiplier</t>
+  </si>
+  <si>
+    <t>Dark Resist</t>
+  </si>
+  <si>
+    <t>Dark Resist Multiplier</t>
+  </si>
+  <si>
+    <t>Resist All</t>
+  </si>
+  <si>
+    <t>Resist All Multiplier</t>
+  </si>
+  <si>
+    <t>Stat Multiplier</t>
   </si>
 </sst>
 </file>
@@ -773,13 +785,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V62"/>
+  <dimension ref="A1:X62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D63" sqref="D63"/>
+      <selection pane="bottomRight" activeCell="Y32" sqref="Y32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,10 +815,10 @@
     <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="27" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -847,7 +859,7 @@
         <v>33</v>
       </c>
       <c r="N1" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="O1" t="s">
         <v>43</v>
@@ -856,534 +868,579 @@
         <v>46</v>
       </c>
       <c r="Q1" t="s">
-        <v>102</v>
+        <v>60</v>
       </c>
       <c r="R1" t="s">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="S1" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="T1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" t="s">
+        <v>88</v>
+      </c>
+      <c r="W1" t="s">
+        <v>50</v>
+      </c>
+      <c r="X1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1.05</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>90</v>
+      </c>
+      <c r="X2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="U3" t="s">
+        <v>93</v>
+      </c>
+      <c r="V3" t="s">
         <v>91</v>
       </c>
-      <c r="U1" t="s">
-        <v>86</v>
-      </c>
-      <c r="V1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
+      <c r="X3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1.05</v>
+      </c>
+      <c r="U4" t="s">
+        <v>106</v>
+      </c>
+      <c r="V4" t="s">
+        <v>90</v>
+      </c>
+      <c r="X4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="U5" t="s">
+        <v>107</v>
+      </c>
+      <c r="V5" t="s">
+        <v>91</v>
+      </c>
+      <c r="X5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1.05</v>
+      </c>
+      <c r="U6" t="s">
+        <v>108</v>
+      </c>
+      <c r="V6" t="s">
+        <v>90</v>
+      </c>
+      <c r="X6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="U7" t="s">
+        <v>109</v>
+      </c>
+      <c r="V7" t="s">
+        <v>91</v>
+      </c>
+      <c r="X7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1.05</v>
+      </c>
+      <c r="U8" t="s">
+        <v>110</v>
+      </c>
+      <c r="V8" t="s">
+        <v>90</v>
+      </c>
+      <c r="X8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="U9" t="s">
+        <v>111</v>
+      </c>
+      <c r="V9" t="s">
+        <v>91</v>
+      </c>
+      <c r="X9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
         <v>100</v>
-      </c>
-      <c r="T2">
-        <v>1.01</v>
-      </c>
-      <c r="U2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>100</v>
-      </c>
-      <c r="R3" t="b">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>1.01</v>
-      </c>
-      <c r="U3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4" t="b">
-        <v>1</v>
-      </c>
-      <c r="R4" t="b">
-        <v>1</v>
-      </c>
-      <c r="T4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>5</v>
-      </c>
-      <c r="R5" t="b">
-        <v>1</v>
-      </c>
-      <c r="T5">
-        <v>1.01</v>
-      </c>
-      <c r="U5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6" t="b">
-        <v>1</v>
-      </c>
-      <c r="R6" t="b">
-        <v>1</v>
-      </c>
-      <c r="T6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>10</v>
-      </c>
-      <c r="T7">
-        <v>1.01</v>
-      </c>
-      <c r="U7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <v>10</v>
-      </c>
-      <c r="R8" t="b">
-        <v>1</v>
-      </c>
-      <c r="T8">
-        <v>1.01</v>
-      </c>
-      <c r="U8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9" t="b">
-        <v>1</v>
-      </c>
-      <c r="R9" t="b">
-        <v>1</v>
-      </c>
-      <c r="T9">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <v>5</v>
-      </c>
-      <c r="R10" t="b">
-        <v>1</v>
       </c>
       <c r="T10">
         <v>1.01</v>
       </c>
-      <c r="U10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1425,641 +1482,710 @@
         <v>1</v>
       </c>
       <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="P11" t="b">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="R11" t="b">
         <v>1</v>
       </c>
       <c r="T11">
+        <v>1.01</v>
+      </c>
+      <c r="U11" t="s">
+        <v>94</v>
+      </c>
+      <c r="V11" t="s">
+        <v>90</v>
+      </c>
+      <c r="X11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U12" t="s">
+        <v>95</v>
+      </c>
+      <c r="V12" t="s">
+        <v>91</v>
+      </c>
+      <c r="X12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>5</v>
+      </c>
+      <c r="R13" t="b">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>1.01</v>
+      </c>
+      <c r="U13" t="s">
+        <v>96</v>
+      </c>
+      <c r="V13" t="s">
+        <v>92</v>
+      </c>
+      <c r="X13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14" t="b">
+        <v>1</v>
+      </c>
+      <c r="R14" t="b">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="U14" t="s">
+        <v>97</v>
+      </c>
+      <c r="V14" t="s">
+        <v>91</v>
+      </c>
+      <c r="X14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>10</v>
+      </c>
+      <c r="T15">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>10</v>
+      </c>
+      <c r="R16" t="b">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>1.01</v>
+      </c>
+      <c r="U16" t="s">
+        <v>98</v>
+      </c>
+      <c r="V16" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="X16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17" t="b">
+        <v>1</v>
+      </c>
+      <c r="R17" t="b">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="U17" t="s">
+        <v>99</v>
+      </c>
+      <c r="V17" t="s">
+        <v>91</v>
+      </c>
+      <c r="X17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>5</v>
+      </c>
+      <c r="R18" t="b">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1.01</v>
+      </c>
+      <c r="U18" t="s">
+        <v>100</v>
+      </c>
+      <c r="V18" t="s">
+        <v>92</v>
+      </c>
+      <c r="X18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19" t="b">
+        <v>1</v>
+      </c>
+      <c r="R19" t="b">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="U19" t="s">
+        <v>101</v>
+      </c>
+      <c r="V19" t="s">
+        <v>91</v>
+      </c>
+      <c r="X19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="R12" t="b">
-        <v>1</v>
-      </c>
-      <c r="T12">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="R20" t="b">
+        <v>1</v>
+      </c>
+      <c r="T20">
         <v>1.25</v>
       </c>
-      <c r="U12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="U20" t="s">
+        <v>102</v>
+      </c>
+      <c r="V20" t="s">
+        <v>90</v>
+      </c>
+      <c r="X20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="R13" t="b">
-        <v>1</v>
-      </c>
-      <c r="T13">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="R21" t="b">
+        <v>1</v>
+      </c>
+      <c r="T21">
         <v>1.25</v>
       </c>
-      <c r="U13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="U21" t="s">
+        <v>103</v>
+      </c>
+      <c r="V21" t="s">
+        <v>90</v>
+      </c>
+      <c r="X21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>14</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14">
-        <v>1</v>
-      </c>
-      <c r="P14" t="b">
-        <v>1</v>
-      </c>
-      <c r="R14" t="b">
-        <v>1</v>
-      </c>
-      <c r="T14">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22" t="b">
+        <v>1</v>
+      </c>
+      <c r="R22" t="b">
+        <v>1</v>
+      </c>
+      <c r="T22">
         <v>1.3</v>
       </c>
-      <c r="U14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15">
-        <v>1</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="Q15" t="b">
-        <v>1</v>
-      </c>
-      <c r="T15">
-        <v>1.05</v>
-      </c>
-      <c r="U15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="N16">
-        <v>1</v>
-      </c>
-      <c r="O16">
-        <v>1</v>
-      </c>
-      <c r="P16" t="b">
-        <v>1</v>
-      </c>
-      <c r="T16">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="U16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
-      <c r="O17">
-        <v>1</v>
-      </c>
-      <c r="Q17" t="b">
-        <v>1</v>
-      </c>
-      <c r="T17">
-        <v>1.05</v>
-      </c>
-      <c r="U17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-      <c r="N18">
-        <v>1</v>
-      </c>
-      <c r="O18">
-        <v>1</v>
-      </c>
-      <c r="P18" t="b">
-        <v>1</v>
-      </c>
-      <c r="T18">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="U18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
-      <c r="N19">
-        <v>1</v>
-      </c>
-      <c r="O19">
-        <v>1</v>
-      </c>
-      <c r="Q19" t="b">
-        <v>1</v>
-      </c>
-      <c r="T19">
-        <v>1.05</v>
-      </c>
-      <c r="U19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
-      <c r="N20">
-        <v>1</v>
-      </c>
-      <c r="O20">
-        <v>1</v>
-      </c>
-      <c r="P20" t="b">
-        <v>1</v>
-      </c>
-      <c r="T20">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="U20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-      <c r="O21">
-        <v>1</v>
-      </c>
-      <c r="R21" t="b">
-        <v>1</v>
-      </c>
-      <c r="T21">
-        <v>1.05</v>
-      </c>
-      <c r="U21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-      <c r="K22">
-        <v>1</v>
-      </c>
-      <c r="L22">
-        <v>1</v>
-      </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="O22">
-        <v>1</v>
-      </c>
-      <c r="P22" t="b">
-        <v>1</v>
-      </c>
-      <c r="T22">
-        <v>1.1499999999999999</v>
-      </c>
       <c r="U22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="V22" t="s">
+        <v>91</v>
+      </c>
+      <c r="X22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -2109,10 +2235,16 @@
         <v>1.01</v>
       </c>
       <c r="U23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="V23" t="s">
+        <v>90</v>
+      </c>
+      <c r="X23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -2168,10 +2300,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="V24" t="s">
+        <v>91</v>
+      </c>
+      <c r="X24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -2221,10 +2359,16 @@
         <v>1.02</v>
       </c>
       <c r="U25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="V25" t="s">
+        <v>90</v>
+      </c>
+      <c r="X25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -2277,10 +2421,16 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="U26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="V26" t="s">
+        <v>91</v>
+      </c>
+      <c r="X26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2330,10 +2480,16 @@
         <v>1.2</v>
       </c>
       <c r="U27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="V27" t="s">
+        <v>90</v>
+      </c>
+      <c r="X27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -2389,10 +2545,16 @@
         <v>1.2</v>
       </c>
       <c r="U28" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="V28" t="s">
+        <v>91</v>
+      </c>
+      <c r="X28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2448,10 +2610,16 @@
         <v>1.3</v>
       </c>
       <c r="U29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="V29" t="s">
+        <v>91</v>
+      </c>
+      <c r="X29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -2501,10 +2669,16 @@
         <v>1.02</v>
       </c>
       <c r="U30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="V30" t="s">
+        <v>90</v>
+      </c>
+      <c r="X30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -2557,10 +2731,16 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="U31" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="V31" t="s">
+        <v>91</v>
+      </c>
+      <c r="X31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -2616,10 +2796,16 @@
         <v>1.02</v>
       </c>
       <c r="U32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="V32" t="s">
+        <v>91</v>
+      </c>
+      <c r="X32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -2672,10 +2858,16 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="U33" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="V33" t="s">
+        <v>91</v>
+      </c>
+      <c r="X33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -2731,10 +2923,16 @@
         <v>1.05</v>
       </c>
       <c r="U34" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="V34" t="s">
+        <v>90</v>
+      </c>
+      <c r="X34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -2787,12 +2985,18 @@
         <v>1.2</v>
       </c>
       <c r="U35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="V35" t="s">
+        <v>91</v>
+      </c>
+      <c r="X35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -2846,12 +3050,18 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U36" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="V36" t="s">
+        <v>90</v>
+      </c>
+      <c r="X36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -2905,12 +3115,18 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U37" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="V37" t="s">
+        <v>91</v>
+      </c>
+      <c r="X37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2961,12 +3177,18 @@
         <v>1.05</v>
       </c>
       <c r="U38" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="V38" t="s">
+        <v>90</v>
+      </c>
+      <c r="X38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -3017,12 +3239,18 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="U39" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="V39" t="s">
+        <v>91</v>
+      </c>
+      <c r="X39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -3073,12 +3301,18 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U40" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="V40" t="s">
+        <v>91</v>
+      </c>
+      <c r="X40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -3129,12 +3363,18 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U41" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="V41" t="s">
+        <v>91</v>
+      </c>
+      <c r="X41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -3185,12 +3425,18 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U42" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="V42" t="s">
+        <v>91</v>
+      </c>
+      <c r="X42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -3241,12 +3487,18 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U43" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="V43" t="s">
+        <v>91</v>
+      </c>
+      <c r="X43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>75</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -3300,12 +3552,18 @@
         <v>1.05</v>
       </c>
       <c r="U44" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="V44" t="s">
+        <v>91</v>
+      </c>
+      <c r="X44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>141</v>
+        <v>81</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -3359,12 +3617,18 @@
         <v>1.05</v>
       </c>
       <c r="U45" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="V45" t="s">
+        <v>91</v>
+      </c>
+      <c r="X45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>120</v>
+        <v>76</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -3418,12 +3682,18 @@
         <v>1.05</v>
       </c>
       <c r="U46" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="V46" t="s">
+        <v>91</v>
+      </c>
+      <c r="X46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -3477,12 +3747,18 @@
         <v>1.05</v>
       </c>
       <c r="U47" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="V47" t="s">
+        <v>91</v>
+      </c>
+      <c r="X47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -3533,12 +3809,18 @@
         <v>1.05</v>
       </c>
       <c r="U48" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="V48" t="s">
+        <v>90</v>
+      </c>
+      <c r="X48" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -3589,12 +3871,18 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U49" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="V49" t="s">
+        <v>91</v>
+      </c>
+      <c r="X49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>138</v>
+        <v>78</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -3645,12 +3933,18 @@
         <v>1.05</v>
       </c>
       <c r="U50" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="V50" t="s">
+        <v>90</v>
+      </c>
+      <c r="X50" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -3701,12 +3995,18 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U51" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="V51" t="s">
+        <v>91</v>
+      </c>
+      <c r="X51" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -3757,12 +4057,18 @@
         <v>1.05</v>
       </c>
       <c r="U52" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="V52" t="s">
+        <v>90</v>
+      </c>
+      <c r="X52" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>114</v>
+        <v>70</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -3813,12 +4119,18 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U53" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="V53" t="s">
+        <v>91</v>
+      </c>
+      <c r="X53" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -3869,12 +4181,18 @@
         <v>1.05</v>
       </c>
       <c r="U54" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="V54" t="s">
+        <v>90</v>
+      </c>
+      <c r="X54" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -3925,12 +4243,18 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U55" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="V55" t="s">
+        <v>91</v>
+      </c>
+      <c r="X55" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -3981,12 +4305,18 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="U56" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="V56" t="s">
+        <v>90</v>
+      </c>
+      <c r="X56" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="P57" t="b">
         <v>1</v>
@@ -3995,12 +4325,18 @@
         <v>1.25</v>
       </c>
       <c r="U57" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="V57" t="s">
+        <v>91</v>
+      </c>
+      <c r="X57" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="O58">
         <v>1</v>
@@ -4012,39 +4348,33 @@
         <v>1.4</v>
       </c>
       <c r="U58" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="V58" t="s">
+        <v>91</v>
+      </c>
+      <c r="X58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>47</v>
       </c>
-      <c r="U59" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>48</v>
       </c>
-      <c r="U60" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>49</v>
       </c>
-      <c r="U61" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>99</v>
-      </c>
-      <c r="U62" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tooltip support - Added dynamic tooltip support - Preparation for proper item tooltips
</commit_message>
<xml_diff>
--- a/data/content/Stats.xlsx
+++ b/data/content/Stats.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\SMC\EndlessBattleFC\data\content\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="24180" yWindow="0" windowWidth="18000" windowHeight="18240"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="152">
   <si>
     <t>name</t>
   </si>
@@ -466,6 +471,15 @@
   </si>
   <si>
     <t>canSpendStatPoints</t>
+  </si>
+  <si>
+    <t>Increases Attack Damage</t>
+  </si>
+  <si>
+    <t>Multiplies your Strength Attribute</t>
+  </si>
+  <si>
+    <t>Your Character's Hitpoints</t>
   </si>
 </sst>
 </file>
@@ -775,7 +789,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -789,7 +803,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y9" sqref="Y9"/>
+      <selection pane="bottomRight" activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,6 +965,9 @@
       <c r="V2" t="s">
         <v>90</v>
       </c>
+      <c r="W2" t="s">
+        <v>149</v>
+      </c>
       <c r="X2" t="s">
         <v>83</v>
       </c>
@@ -1016,6 +1033,9 @@
       <c r="V3" t="s">
         <v>91</v>
       </c>
+      <c r="W3" t="s">
+        <v>150</v>
+      </c>
       <c r="X3" t="s">
         <v>87</v>
       </c>
@@ -1508,6 +1528,9 @@
       </c>
       <c r="V11" t="s">
         <v>90</v>
+      </c>
+      <c r="W11" t="s">
+        <v>151</v>
       </c>
       <c r="X11" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Updating the stats table with rebalancing
</commit_message>
<xml_diff>
--- a/data/content/Stats.xlsx
+++ b/data/content/Stats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="186">
   <si>
     <t>name</t>
   </si>
@@ -122,6 +122,18 @@
     <t>Extra</t>
   </si>
   <si>
+    <t>strAff</t>
+  </si>
+  <si>
+    <t>Strength Affinity</t>
+  </si>
+  <si>
+    <t>Your character's affinity to Strength</t>
+  </si>
+  <si>
+    <t>Affinity</t>
+  </si>
+  <si>
     <t>agi</t>
   </si>
   <si>
@@ -140,6 +152,15 @@
     <t>Multiplies your Agiligy Attribute</t>
   </si>
   <si>
+    <t>agiAff</t>
+  </si>
+  <si>
+    <t>Agility Affinity</t>
+  </si>
+  <si>
+    <t>Your character's affinity to Agility</t>
+  </si>
+  <si>
     <t>int</t>
   </si>
   <si>
@@ -158,6 +179,15 @@
     <t>Multiplies your Intelligence Attribute</t>
   </si>
   <si>
+    <t>intAff</t>
+  </si>
+  <si>
+    <t>Intelligence Affinity</t>
+  </si>
+  <si>
+    <t>Your character's affinity to Intelligence</t>
+  </si>
+  <si>
     <t>sta</t>
   </si>
   <si>
@@ -174,6 +204,15 @@
   </si>
   <si>
     <t>Multiplies your Stamina Attribute</t>
+  </si>
+  <si>
+    <t>staAff</t>
+  </si>
+  <si>
+    <t>Stamina Affinity</t>
+  </si>
+  <si>
+    <t>Your character's affinity to Stamina</t>
   </si>
   <si>
     <t>hp</t>
@@ -631,14 +670,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y63"/>
+  <dimension ref="A1:Y67"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
-      <selection pane="bottomRight" activeCell="A63" activeCellId="0" sqref="A63"/>
+      <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="Y12" activeCellId="0" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -663,8 +702,10 @@
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.8571428571429"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="27"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="31.7040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="8.70918367346939"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="43.1632653061225"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.5408163265306"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="13.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.70918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,7 +785,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>25</v>
       </c>
@@ -808,10 +849,6 @@
       </c>
       <c r="X2" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="Y2" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -880,59 +917,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="T4" s="0" t="n">
-        <v>1.05</v>
-      </c>
       <c r="U4" s="0" t="s">
         <v>36</v>
       </c>
@@ -943,82 +931,81 @@
         <v>37</v>
       </c>
       <c r="X4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="X5" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="Y4" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P5" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="T5" s="0" t="n">
-        <v>1.15</v>
-      </c>
-      <c r="U5" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="V5" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="W5" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="X5" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -1062,99 +1049,49 @@
       <c r="O6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="Q6" s="0" t="n">
+      <c r="P6" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T6" s="0" t="n">
-        <v>1.05</v>
+        <v>1.15</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="V7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="W6" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="X6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y6" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P7" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="T7" s="0" t="n">
-        <v>1.15</v>
-      </c>
-      <c r="U7" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="V7" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="W7" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="X7" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
@@ -1198,7 +1135,7 @@
       <c r="O8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="R8" s="0" t="n">
+      <c r="Q8" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1206,25 +1143,21 @@
         <v>1.05</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="V8" s="0" t="s">
         <v>27</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="X8" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="Y8" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -1276,74 +1209,41 @@
         <v>1.15</v>
       </c>
       <c r="U9" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="V9" s="0" t="s">
         <v>32</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="X9" s="0" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O10" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="T10" s="0" t="n">
-        <v>1.01</v>
+        <v>54</v>
+      </c>
+      <c r="U10" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="V10" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+      <c r="X10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -1385,31 +1285,31 @@
         <v>1</v>
       </c>
       <c r="O11" s="0" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="R11" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T11" s="0" t="n">
-        <v>1.01</v>
+        <v>1.05</v>
       </c>
       <c r="U11" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V11" s="0" t="s">
         <v>27</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="X11" s="0" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
@@ -1457,90 +1357,40 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="R12" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="T12" s="0" t="n">
-        <v>1.1</v>
+        <v>1.15</v>
       </c>
       <c r="U12" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="V12" s="0" t="s">
         <v>32</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="X12" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O13" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="R13" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="T13" s="0" t="n">
-        <v>1.01</v>
+        <v>63</v>
       </c>
       <c r="U13" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="V13" s="0" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="W13" s="0" t="s">
         <v>65</v>
       </c>
       <c r="X13" s="0" t="s">
-        <v>58</v>
+        <v>38</v>
+      </c>
+      <c r="Y13" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,35 +1437,18 @@
         <v>1</v>
       </c>
       <c r="O14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P14" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R14" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="T14" s="0" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="U14" s="0" t="s">
+        <v>1.01</v>
+      </c>
+      <c r="W14" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="V14" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="W14" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="X14" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -1657,82 +1490,99 @@
         <v>1</v>
       </c>
       <c r="O15" s="0" t="n">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="T15" s="0" t="n">
         <v>1.01</v>
       </c>
+      <c r="U15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="V15" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="W15" s="0" t="s">
         <v>70</v>
       </c>
+      <c r="X15" s="0" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="U16" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="V16" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="W16" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="X16" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O16" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="R16" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="T16" s="0" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="U16" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="V16" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="W16" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="X16" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>75</v>
       </c>
@@ -1776,35 +1626,31 @@
         <v>1</v>
       </c>
       <c r="O17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P17" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R17" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T17" s="0" t="n">
-        <v>1.1</v>
+        <v>1.01</v>
       </c>
       <c r="U17" s="0" t="s">
         <v>76</v>
       </c>
       <c r="V17" s="0" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="W17" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="X17" s="0" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
@@ -1846,31 +1692,35 @@
         <v>1</v>
       </c>
       <c r="O18" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="R18" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T18" s="0" t="n">
-        <v>1.01</v>
+        <v>1.1</v>
       </c>
       <c r="U18" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="V18" s="0" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="W18" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="X18" s="0" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1</v>
@@ -1912,30 +1762,13 @@
         <v>1</v>
       </c>
       <c r="O19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P19" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="R19" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="T19" s="0" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="U19" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="V19" s="0" t="s">
-        <v>32</v>
+        <v>1.01</v>
       </c>
       <c r="W19" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="X19" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,14 +1815,14 @@
         <v>1</v>
       </c>
       <c r="O20" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R20" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T20" s="0" t="n">
-        <v>1.25</v>
+        <v>1.01</v>
       </c>
       <c r="U20" s="0" t="s">
         <v>85</v>
@@ -2001,78 +1834,82 @@
         <v>86</v>
       </c>
       <c r="X20" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="R21" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="T21" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="U21" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="V21" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="W21" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="X21" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R21" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="T21" s="0" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="U21" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="V21" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="W21" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="X21" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -2114,35 +1951,31 @@
         <v>1</v>
       </c>
       <c r="O22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P22" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R22" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T22" s="0" t="n">
-        <v>1.3</v>
+        <v>1.01</v>
       </c>
       <c r="U22" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="V22" s="0" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="W22" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="X22" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>1</v>
@@ -2183,29 +2016,36 @@
       <c r="N23" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="O23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P23" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="R23" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T23" s="0" t="n">
-        <v>1.01</v>
+        <v>1.1</v>
       </c>
       <c r="U23" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="V23" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="W23" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="X23" s="0" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1</v>
@@ -2249,33 +2089,29 @@
       <c r="O24" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="P24" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="R24" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T24" s="0" t="n">
-        <v>1.1</v>
+        <v>1.25</v>
       </c>
       <c r="U24" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="V24" s="0" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="W24" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="X24" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>1</v>
@@ -2316,26 +2152,32 @@
       <c r="N25" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="O25" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R25" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T25" s="0" t="n">
-        <v>1.02</v>
+        <v>1.25</v>
       </c>
       <c r="U25" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="V25" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="W25" s="0" t="s">
+        <v>102</v>
+      </c>
       <c r="X25" s="0" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>1</v>
@@ -2383,22 +2225,29 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="R26" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="T26" s="0" t="n">
-        <v>1.11</v>
+        <v>1.3</v>
       </c>
       <c r="U26" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="V26" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="W26" s="0" t="s">
+        <v>105</v>
+      </c>
       <c r="X26" s="0" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>1</v>
@@ -2439,26 +2288,29 @@
       <c r="N27" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S27" s="0" t="n">
+      <c r="R27" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T27" s="0" t="n">
-        <v>1.2</v>
+        <v>1.01</v>
       </c>
       <c r="U27" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="V27" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="W27" s="0" t="s">
+        <v>108</v>
+      </c>
       <c r="X27" s="0" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>1</v>
@@ -2506,26 +2358,29 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="S28" s="0" t="n">
+      <c r="R28" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T28" s="0" t="n">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="U28" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="V28" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="W28" s="0" t="s">
+        <v>111</v>
+      </c>
       <c r="X28" s="0" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1</v>
@@ -2566,33 +2421,26 @@
       <c r="N29" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P29" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="S29" s="0" t="n">
+      <c r="R29" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T29" s="0" t="n">
-        <v>1.3</v>
+        <v>1.02</v>
       </c>
       <c r="U29" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="V29" s="0" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="X29" s="0" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
@@ -2633,26 +2481,29 @@
       <c r="N30" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="R30" s="0" t="n">
+      <c r="O30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P30" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T30" s="0" t="n">
-        <v>1.02</v>
+        <v>1.11</v>
       </c>
       <c r="U30" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="V30" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="X30" s="0" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
@@ -2693,29 +2544,26 @@
       <c r="N31" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P31" s="0" t="n">
+      <c r="S31" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T31" s="0" t="n">
-        <v>1.11</v>
+        <v>1.2</v>
       </c>
       <c r="U31" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="V31" s="0" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="X31" s="0" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -2757,32 +2605,32 @@
         <v>1</v>
       </c>
       <c r="O32" s="0" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="P32" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="R32" s="0" t="n">
+      <c r="S32" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T32" s="0" t="n">
-        <v>1.02</v>
+        <v>1.2</v>
       </c>
       <c r="U32" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="V32" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X32" s="0" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
@@ -2830,22 +2678,26 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="S33" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="T33" s="0" t="n">
-        <v>1.11</v>
+        <v>1.3</v>
       </c>
       <c r="U33" s="0" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="V33" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X33" s="0" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
@@ -2886,32 +2738,26 @@
       <c r="N34" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P34" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R34" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T34" s="0" t="n">
-        <v>1.05</v>
+        <v>1.02</v>
       </c>
       <c r="U34" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="V34" s="0" t="s">
         <v>27</v>
       </c>
       <c r="X34" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
@@ -2960,21 +2806,21 @@
         <v>1</v>
       </c>
       <c r="T35" s="0" t="n">
-        <v>1.2</v>
+        <v>1.11</v>
       </c>
       <c r="U35" s="0" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="V35" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X35" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
@@ -3016,32 +2862,32 @@
         <v>1</v>
       </c>
       <c r="O36" s="0" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="P36" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="S36" s="0" t="n">
+      <c r="R36" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T36" s="0" t="n">
-        <v>1.1</v>
+        <v>1.02</v>
       </c>
       <c r="U36" s="0" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="V36" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="X36" s="0" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
@@ -3089,26 +2935,22 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="S37" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="T37" s="0" t="n">
-        <v>1.1</v>
+        <v>1.11</v>
       </c>
       <c r="U37" s="0" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="V37" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X37" s="0" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -3150,6 +2992,9 @@
         <v>1</v>
       </c>
       <c r="O38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P38" s="0" t="n">
         <v>1</v>
       </c>
       <c r="R38" s="0" t="n">
@@ -3160,18 +3005,18 @@
         <v>1.05</v>
       </c>
       <c r="U38" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="V38" s="0" t="s">
         <v>27</v>
       </c>
       <c r="X38" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
@@ -3220,21 +3065,21 @@
         <v>1</v>
       </c>
       <c r="T39" s="0" t="n">
-        <v>1.15</v>
+        <v>1.2</v>
       </c>
       <c r="U39" s="0" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="V39" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X39" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1</v>
@@ -3279,6 +3124,10 @@
         <v>1</v>
       </c>
       <c r="P40" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S40" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3286,18 +3135,18 @@
         <v>1.1</v>
       </c>
       <c r="U40" s="0" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="V40" s="0" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="X40" s="0" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1</v>
@@ -3342,6 +3191,10 @@
         <v>1</v>
       </c>
       <c r="P41" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S41" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3349,18 +3202,18 @@
         <v>1.1</v>
       </c>
       <c r="U41" s="0" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="V41" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X41" s="0" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
@@ -3404,26 +3257,26 @@
       <c r="O42" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="P42" s="0" t="n">
+      <c r="R42" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T42" s="0" t="n">
-        <v>1.1</v>
+        <v>1.05</v>
       </c>
       <c r="U42" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="V42" s="0" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="X42" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1</v>
@@ -3472,21 +3325,21 @@
         <v>1</v>
       </c>
       <c r="T43" s="0" t="n">
-        <v>1.1</v>
+        <v>1.15</v>
       </c>
       <c r="U43" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="V43" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X43" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>1</v>
@@ -3534,26 +3387,22 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="R44" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="T44" s="0" t="n">
-        <v>1.05</v>
+        <v>1.1</v>
       </c>
       <c r="U44" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="V44" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X44" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1</v>
@@ -3601,26 +3450,22 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="R45" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="T45" s="0" t="n">
-        <v>1.05</v>
+        <v>1.1</v>
       </c>
       <c r="U45" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="V45" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X45" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
@@ -3668,26 +3513,22 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="R46" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="T46" s="0" t="n">
-        <v>1.05</v>
+        <v>1.1</v>
       </c>
       <c r="U46" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="V46" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X46" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>1</v>
@@ -3735,26 +3576,22 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="R47" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
       <c r="T47" s="0" t="n">
-        <v>1.05</v>
+        <v>1.1</v>
       </c>
       <c r="U47" s="0" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="V47" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X47" s="0" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1</v>
@@ -3796,6 +3633,10 @@
         <v>1</v>
       </c>
       <c r="O48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P48" s="0" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="R48" s="0" t="n">
@@ -3806,18 +3647,18 @@
         <v>1.05</v>
       </c>
       <c r="U48" s="0" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="V48" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="X48" s="0" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>1</v>
@@ -3865,22 +3706,26 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="R49" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="T49" s="0" t="n">
-        <v>1.1</v>
+        <v>1.05</v>
       </c>
       <c r="U49" s="0" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="V49" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X49" s="0" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1</v>
@@ -3922,6 +3767,10 @@
         <v>1</v>
       </c>
       <c r="O50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P50" s="0" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="R50" s="0" t="n">
@@ -3932,18 +3781,18 @@
         <v>1.05</v>
       </c>
       <c r="U50" s="0" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="V50" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="X50" s="0" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>1</v>
@@ -3991,22 +3840,26 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="R51" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="T51" s="0" t="n">
-        <v>1.1</v>
+        <v>1.05</v>
       </c>
       <c r="U51" s="0" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="V51" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X51" s="0" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>1</v>
@@ -4058,18 +3911,18 @@
         <v>1.05</v>
       </c>
       <c r="U52" s="0" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="V52" s="0" t="s">
         <v>27</v>
       </c>
       <c r="X52" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>1</v>
@@ -4121,18 +3974,18 @@
         <v>1.1</v>
       </c>
       <c r="U53" s="0" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="V53" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X53" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
@@ -4184,18 +4037,18 @@
         <v>1.05</v>
       </c>
       <c r="U54" s="0" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="V54" s="0" t="s">
         <v>27</v>
       </c>
       <c r="X54" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>1</v>
@@ -4247,18 +4100,18 @@
         <v>1.1</v>
       </c>
       <c r="U55" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="V55" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X55" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>1</v>
@@ -4307,86 +4160,338 @@
         <v>1</v>
       </c>
       <c r="T56" s="0" t="n">
-        <v>1.15</v>
+        <v>1.05</v>
       </c>
       <c r="U56" s="0" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="V56" s="0" t="s">
         <v>27</v>
       </c>
       <c r="X56" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O57" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="P57" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T57" s="0" t="n">
-        <v>1.25</v>
+        <v>1.1</v>
       </c>
       <c r="U57" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="V57" s="0" t="s">
         <v>32</v>
       </c>
       <c r="X57" s="0" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>166</v>
+        <v>171</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N58" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="O58" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="P58" s="0" t="n">
+      <c r="R58" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="T58" s="0" t="n">
-        <v>1.4</v>
+        <v>1.05</v>
       </c>
       <c r="U58" s="0" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="V58" s="0" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="X58" s="0" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>168</v>
+        <v>173</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P59" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="T59" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="U59" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="V59" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="X59" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>169</v>
+        <v>175</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R60" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="T60" s="0" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="U60" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="V60" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="X60" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>170</v>
+        <v>177</v>
+      </c>
+      <c r="P61" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="T61" s="0" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="U61" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="V61" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="X61" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>179</v>
+      </c>
+      <c r="O62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P62" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="T62" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="U62" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="V62" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="X62" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>172</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>